<commit_message>
Modificaciones solicitadas por Félix
</commit_message>
<xml_diff>
--- a/Prueba.xlsx
+++ b/Prueba.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,13 +11,21 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211" fullCalcOnLoad="1"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>Columna 1</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,11 +62,16 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -343,36 +356,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>